<commit_message>
updated coha top decades
</commit_message>
<xml_diff>
--- a/coha_decades/coha_top_decades.xlsx
+++ b/coha_decades/coha_top_decades.xlsx
@@ -265,14 +265,27 @@
     <t>Data: Corpus of Historical American English, Brigham Young University (http://corpus.byu.edu/coha/)</t>
   </si>
   <si>
-    <t>Methodology: Overly common words (appearing in 16 or more decades), as were proper nouns (words that did not appear in a Scrabble dictionary)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code: </t>
+    <t>Code: http://github.com/Prooffreader/word_list_tools (coha_decades folder)</t>
+  </si>
+  <si>
+    <t>Methodology: Overly common words (those appearing in 16 or more decades) and proper nouns (those that did not appear in a Scrabble dictionary) were omitted</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Decade specificity </t>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="CorisandeRegular"/>
+      </rPr>
+      <t>Decade specificity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="CorisandeRegular"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -306,9 +319,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode=";;"/>
+    <numFmt numFmtId="164" formatCode=";;"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +513,11 @@
     <font>
       <sz val="9"/>
       <color rgb="FF00B050"/>
+      <name val="CorisandeRegular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="CorisandeRegular"/>
     </font>
   </fonts>
@@ -895,15 +913,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -912,12 +930,12 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -926,12 +944,12 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -940,49 +958,25 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment textRotation="60"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="27" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1002,8 +996,32 @@
     <xf numFmtId="1" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1049,18 +1067,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1340,114 +1351,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE64"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AE63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:AE60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11:AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="1.42578125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="1.42578125" style="24" customWidth="1"/>
     <col min="5" max="5" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="1.85546875" style="25" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="1.140625" style="1" customWidth="1"/>
     <col min="10" max="29" width="3" style="2" customWidth="1"/>
     <col min="30" max="31" width="2.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="30.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
     </row>
-    <row r="3" spans="1:31" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:31" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="29"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="24" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="26"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="32" t="s">
+      <c r="I4" s="26"/>
+      <c r="J4" s="28" t="s">
         <v>71</v>
       </c>
       <c r="K4" s="9"/>
@@ -1473,75 +1487,75 @@
       <c r="AE4"/>
     </row>
     <row r="5" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="46" t="s">
+      <c r="A5" s="43"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="26" t="s">
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="L5" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="M5" s="26" t="s">
+      <c r="M5" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="N5" s="26" t="s">
+      <c r="N5" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="O5" s="26" t="s">
+      <c r="O5" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="26" t="s">
+      <c r="P5" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="Q5" s="26" t="s">
+      <c r="Q5" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="R5" s="26" t="s">
+      <c r="R5" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="S5" s="26" t="s">
+      <c r="S5" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="T5" s="26" t="s">
+      <c r="T5" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="U5" s="26" t="s">
+      <c r="U5" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="V5" s="26" t="s">
+      <c r="V5" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="W5" s="26" t="s">
+      <c r="W5" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="X5" s="26" t="s">
+      <c r="X5" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="Y5" s="26" t="s">
+      <c r="Y5" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="Z5" s="26" t="s">
+      <c r="Z5" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="AA5" s="26" t="s">
+      <c r="AA5" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="AB5" s="26" t="s">
+      <c r="AB5" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="AC5" s="26" t="s">
+      <c r="AC5" s="25" t="s">
         <v>69</v>
       </c>
       <c r="AD5"/>
@@ -1551,14 +1565,14 @@
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="31">
         <v>1334.8499893037599</v>
       </c>
       <c r="C6" s="12">
         <v>1334.8499893037599</v>
       </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="42">
+      <c r="E6" s="34">
         <v>111.23749910864599</v>
       </c>
       <c r="F6" s="16">
@@ -1636,14 +1650,14 @@
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="32">
         <v>1021.6116434015401</v>
       </c>
       <c r="C7" s="10">
         <v>1021.6116434015401</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="43">
+      <c r="E7" s="35">
         <v>78.585511030888199</v>
       </c>
       <c r="F7" s="6">
@@ -1721,14 +1735,14 @@
       <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="32">
         <v>1063.24213783902</v>
       </c>
       <c r="C8" s="10">
         <v>1063.24213783902</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="43">
+      <c r="E8" s="35">
         <v>75.945866988502004</v>
       </c>
       <c r="F8" s="6">
@@ -1806,14 +1820,14 @@
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="32">
         <v>715.25355866289397</v>
       </c>
       <c r="C9" s="10">
         <v>715.25355866289397</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="43">
+      <c r="E9" s="35">
         <v>65.023050787535794</v>
       </c>
       <c r="F9" s="6">
@@ -1891,14 +1905,14 @@
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="40">
+      <c r="B10" s="32">
         <v>638.322618809338</v>
       </c>
       <c r="C10" s="10">
         <v>638.322618809338</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="43">
+      <c r="E10" s="35">
         <v>63.8322618809338</v>
       </c>
       <c r="F10" s="6">
@@ -1976,14 +1990,14 @@
       <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="31">
         <v>928.72697699395906</v>
       </c>
       <c r="C11" s="12">
         <v>928.72697699395906</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="E11" s="42">
+      <c r="E11" s="34">
         <v>61.915131799597198</v>
       </c>
       <c r="F11" s="16">
@@ -2061,14 +2075,14 @@
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="40">
+      <c r="B12" s="32">
         <v>565.58995940218506</v>
       </c>
       <c r="C12" s="10">
         <v>565.58995940218506</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="43">
+      <c r="E12" s="35">
         <v>51.417269036562296</v>
       </c>
       <c r="F12" s="6">
@@ -2146,14 +2160,14 @@
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="32">
         <v>623.20970011925704</v>
       </c>
       <c r="C13" s="10">
         <v>623.20970011925704</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="43">
+      <c r="E13" s="35">
         <v>41.547313341283804</v>
       </c>
       <c r="F13" s="6">
@@ -2231,14 +2245,14 @@
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="32">
         <v>476.04687759327896</v>
       </c>
       <c r="C14" s="10">
         <v>476.04687759327896</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="43">
+      <c r="E14" s="35">
         <v>39.670573132773299</v>
       </c>
       <c r="F14" s="6">
@@ -2316,14 +2330,14 @@
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="32">
         <v>453.46201302128702</v>
       </c>
       <c r="C15" s="10">
         <v>453.46201302128702</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="43">
+      <c r="E15" s="35">
         <v>37.7885010851072</v>
       </c>
       <c r="F15" s="6">
@@ -2401,14 +2415,14 @@
       <c r="A16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="39">
+      <c r="B16" s="31">
         <v>531.10669840776507</v>
       </c>
       <c r="C16" s="12">
         <v>531.10669840776507</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="42">
+      <c r="E16" s="34">
         <v>35.407113227184297</v>
       </c>
       <c r="F16" s="16">
@@ -2486,14 +2500,14 @@
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="32">
         <v>314.93351589005596</v>
       </c>
       <c r="C17" s="10">
         <v>314.93351589005596</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="43">
+      <c r="E17" s="35">
         <v>34.992612876672901</v>
       </c>
       <c r="F17" s="6">
@@ -2571,14 +2585,14 @@
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="32">
         <v>381.49570222168001</v>
       </c>
       <c r="C18" s="10">
         <v>381.49570222168001</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="43">
+      <c r="E18" s="35">
         <v>29.345823247821503</v>
       </c>
       <c r="F18" s="6">
@@ -2656,14 +2670,14 @@
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="32">
         <v>438.34569723946601</v>
       </c>
       <c r="C19" s="10">
         <v>438.34569723946601</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="43">
+      <c r="E19" s="35">
         <v>29.223046482631101</v>
       </c>
       <c r="F19" s="6">
@@ -2741,14 +2755,14 @@
       <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="40">
+      <c r="B20" s="32">
         <v>84.830439742664311</v>
       </c>
       <c r="C20" s="6">
         <v>84.830439742664311</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="43">
+      <c r="E20" s="35">
         <v>28.276813247554703</v>
       </c>
       <c r="F20" s="6">
@@ -2826,14 +2840,14 @@
       <c r="A21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="39">
+      <c r="B21" s="31">
         <v>304.64438992403296</v>
       </c>
       <c r="C21" s="16">
         <v>304.64438992403296</v>
       </c>
       <c r="D21" s="13"/>
-      <c r="E21" s="42">
+      <c r="E21" s="34">
         <v>27.694944538548398</v>
       </c>
       <c r="F21" s="16">
@@ -2871,37 +2885,37 @@
       <c r="R21" s="15">
         <v>0</v>
       </c>
-      <c r="S21" s="23">
+      <c r="S21" s="22">
         <v>2.3218736331420099E-5</v>
       </c>
-      <c r="T21" s="23">
+      <c r="T21" s="22">
         <v>2.8963151313956301E-4</v>
       </c>
-      <c r="U21" s="23">
+      <c r="U21" s="22">
         <v>1.33888680528259E-3</v>
       </c>
-      <c r="V21" s="23">
+      <c r="V21" s="22">
         <v>1.5335410854353301E-3</v>
       </c>
-      <c r="W21" s="23">
+      <c r="W21" s="22">
         <v>2.0912370676818E-3</v>
       </c>
-      <c r="X21" s="23">
+      <c r="X21" s="22">
         <v>3.0062967370043099E-3</v>
       </c>
-      <c r="Y21" s="23">
+      <c r="Y21" s="22">
         <v>2.9947937624918799E-3</v>
       </c>
-      <c r="Z21" s="23">
+      <c r="Z21" s="22">
         <v>3.9380863282421899E-3</v>
       </c>
-      <c r="AA21" s="23">
+      <c r="AA21" s="22">
         <v>4.4122360805362599E-3</v>
       </c>
-      <c r="AB21" s="23">
+      <c r="AB21" s="22">
         <v>5.2130816514404403E-3</v>
       </c>
-      <c r="AC21" s="23">
+      <c r="AC21" s="22">
         <v>5.6234292248174902E-3</v>
       </c>
       <c r="AD21"/>
@@ -2911,14 +2925,14 @@
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="32">
         <v>375.68033498045202</v>
       </c>
       <c r="C22" s="6">
         <v>375.68033498045202</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="43">
+      <c r="E22" s="35">
         <v>25.045355665363498</v>
       </c>
       <c r="F22" s="6">
@@ -2996,14 +3010,14 @@
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="40">
+      <c r="B23" s="32">
         <v>275.38432542755402</v>
       </c>
       <c r="C23" s="6">
         <v>275.38432542755402</v>
       </c>
       <c r="D23" s="7"/>
-      <c r="E23" s="43">
+      <c r="E23" s="35">
         <v>22.948693785629498</v>
       </c>
       <c r="F23" s="6">
@@ -3081,14 +3095,14 @@
       <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="32">
         <v>243.62247155908301</v>
       </c>
       <c r="C24" s="6">
         <v>243.62247155908301</v>
       </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="43">
+      <c r="E24" s="35">
         <v>22.147497414462102</v>
       </c>
       <c r="F24" s="6">
@@ -3166,14 +3180,14 @@
       <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="40">
+      <c r="B25" s="32">
         <v>260.51092085279498</v>
       </c>
       <c r="C25" s="6">
         <v>260.51092085279498</v>
       </c>
       <c r="D25" s="7"/>
-      <c r="E25" s="43">
+      <c r="E25" s="35">
         <v>21.709243404399601</v>
       </c>
       <c r="F25" s="6">
@@ -3251,14 +3265,14 @@
       <c r="A26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="39">
+      <c r="B26" s="31">
         <v>321.64909994661105</v>
       </c>
       <c r="C26" s="16">
         <v>321.64909994661105</v>
       </c>
       <c r="D26" s="13"/>
-      <c r="E26" s="42">
+      <c r="E26" s="34">
         <v>21.443273329774001</v>
       </c>
       <c r="F26" s="16">
@@ -3336,14 +3350,14 @@
       <c r="A27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="32">
         <v>272.365844223046</v>
       </c>
       <c r="C27" s="6">
         <v>272.365844223046</v>
       </c>
       <c r="D27" s="7"/>
-      <c r="E27" s="43">
+      <c r="E27" s="35">
         <v>20.9512187863882</v>
       </c>
       <c r="F27" s="6">
@@ -3421,14 +3435,14 @@
       <c r="A28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="40">
+      <c r="B28" s="32">
         <v>277.49606964098899</v>
       </c>
       <c r="C28" s="6">
         <v>277.49606964098899</v>
       </c>
       <c r="D28" s="7"/>
-      <c r="E28" s="43">
+      <c r="E28" s="35">
         <v>19.8211478314992</v>
       </c>
       <c r="F28" s="6">
@@ -3506,14 +3520,14 @@
       <c r="A29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="40">
+      <c r="B29" s="32">
         <v>138.40327711326898</v>
       </c>
       <c r="C29" s="6">
         <v>138.40327711326898</v>
       </c>
       <c r="D29" s="7"/>
-      <c r="E29" s="43">
+      <c r="E29" s="35">
         <v>19.771896730466999</v>
       </c>
       <c r="F29" s="6">
@@ -3591,14 +3605,14 @@
       <c r="A30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="40">
+      <c r="B30" s="32">
         <v>236.147829931822</v>
       </c>
       <c r="C30" s="6">
         <v>236.147829931822</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="43">
+      <c r="E30" s="35">
         <v>19.6789858276518</v>
       </c>
       <c r="F30" s="6">
@@ -3676,14 +3690,14 @@
       <c r="A31" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="39">
+      <c r="B31" s="31">
         <v>291.97865086685397</v>
       </c>
       <c r="C31" s="16">
         <v>291.97865086685397</v>
       </c>
       <c r="D31" s="13"/>
-      <c r="E31" s="42">
+      <c r="E31" s="34">
         <v>19.4652433911236</v>
       </c>
       <c r="F31" s="16">
@@ -3761,14 +3775,14 @@
       <c r="A32" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="40">
+      <c r="B32" s="32">
         <v>193.90763339962001</v>
       </c>
       <c r="C32" s="6">
         <v>193.90763339962001</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="E32" s="43">
+      <c r="E32" s="35">
         <v>19.390763339962</v>
       </c>
       <c r="F32" s="6">
@@ -3846,14 +3860,14 @@
       <c r="A33" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="40">
+      <c r="B33" s="32">
         <v>232.04322909305699</v>
       </c>
       <c r="C33" s="6">
         <v>232.04322909305699</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="E33" s="43">
+      <c r="E33" s="35">
         <v>19.336935757754702</v>
       </c>
       <c r="F33" s="6">
@@ -3931,14 +3945,14 @@
       <c r="A34" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="40">
+      <c r="B34" s="32">
         <v>228.76481389452402</v>
       </c>
       <c r="C34" s="6">
         <v>228.76481389452402</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="43">
+      <c r="E34" s="35">
         <v>19.063734491210298</v>
       </c>
       <c r="F34" s="6">
@@ -4016,14 +4030,14 @@
       <c r="A35" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="40">
+      <c r="B35" s="32">
         <v>17.434045330978101</v>
       </c>
       <c r="C35" s="6">
         <v>17.434045330978101</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="43">
+      <c r="E35" s="35">
         <v>17.434045330978101</v>
       </c>
       <c r="F35" s="6">
@@ -4101,14 +4115,14 @@
       <c r="A36" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="39">
+      <c r="B36" s="31">
         <v>165.88877084000001</v>
       </c>
       <c r="C36" s="16">
         <v>165.88877084000001</v>
       </c>
       <c r="D36" s="13"/>
-      <c r="E36" s="42">
+      <c r="E36" s="34">
         <v>16.588877084</v>
       </c>
       <c r="F36" s="16">
@@ -4186,14 +4200,14 @@
       <c r="A37" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="40">
+      <c r="B37" s="32">
         <v>149.02422097089499</v>
       </c>
       <c r="C37" s="6">
         <v>149.02422097089499</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="43">
+      <c r="E37" s="35">
         <v>16.5582467745439</v>
       </c>
       <c r="F37" s="6">
@@ -4271,14 +4285,14 @@
       <c r="A38" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="40">
+      <c r="B38" s="32">
         <v>16.482605621012201</v>
       </c>
       <c r="C38" s="6">
         <v>16.482605621012201</v>
       </c>
       <c r="D38" s="7"/>
-      <c r="E38" s="43">
+      <c r="E38" s="35">
         <v>16.482605621012201</v>
       </c>
       <c r="F38" s="6">
@@ -4356,14 +4370,14 @@
       <c r="A39" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="40">
+      <c r="B39" s="32">
         <v>16.415730076251002</v>
       </c>
       <c r="C39" s="6">
         <v>16.415730076251002</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="43">
+      <c r="E39" s="35">
         <v>16.415730076251002</v>
       </c>
       <c r="F39" s="6">
@@ -4441,14 +4455,14 @@
       <c r="A40" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="41">
+      <c r="B40" s="33">
         <v>195.128177337783</v>
       </c>
       <c r="C40" s="18">
         <v>195.128177337783</v>
       </c>
       <c r="D40" s="19"/>
-      <c r="E40" s="44">
+      <c r="E40" s="36">
         <v>16.260681444815198</v>
       </c>
       <c r="F40" s="18">
@@ -4526,14 +4540,14 @@
       <c r="A41" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="39">
+      <c r="B41" s="31">
         <v>145.75957943658798</v>
       </c>
       <c r="C41" s="16">
         <v>145.75957943658798</v>
       </c>
       <c r="D41" s="13"/>
-      <c r="E41" s="42">
+      <c r="E41" s="34">
         <v>16.1955088262876</v>
       </c>
       <c r="F41" s="16">
@@ -4574,7 +4588,7 @@
       <c r="S41" s="15">
         <v>0</v>
       </c>
-      <c r="T41" s="23">
+      <c r="T41" s="22">
         <v>4.5254923928056796E-6</v>
       </c>
       <c r="U41" s="15">
@@ -4611,14 +4625,14 @@
       <c r="A42" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="41">
+      <c r="B42" s="33">
         <v>95.570819972817503</v>
       </c>
       <c r="C42" s="18">
         <v>95.570819972817503</v>
       </c>
       <c r="D42" s="19"/>
-      <c r="E42" s="44">
+      <c r="E42" s="36">
         <v>15.9284699954695</v>
       </c>
       <c r="F42" s="18">
@@ -4696,14 +4710,14 @@
       <c r="A43" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="41">
+      <c r="B43" s="33">
         <v>222.12290406155103</v>
       </c>
       <c r="C43" s="18">
         <v>222.12290406155103</v>
       </c>
       <c r="D43" s="19"/>
-      <c r="E43" s="44">
+      <c r="E43" s="36">
         <v>15.865921718682198</v>
       </c>
       <c r="F43" s="18">
@@ -4781,14 +4795,14 @@
       <c r="A44" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="41">
+      <c r="B44" s="33">
         <v>236.81434638992101</v>
       </c>
       <c r="C44" s="18">
         <v>236.81434638992101</v>
       </c>
       <c r="D44" s="19"/>
-      <c r="E44" s="44">
+      <c r="E44" s="36">
         <v>15.7876230926614</v>
       </c>
       <c r="F44" s="18">
@@ -4866,14 +4880,14 @@
       <c r="A45" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="41">
+      <c r="B45" s="33">
         <v>157.456377208459</v>
       </c>
       <c r="C45" s="18">
         <v>157.456377208459</v>
       </c>
       <c r="D45" s="19"/>
-      <c r="E45" s="44">
+      <c r="E45" s="36">
         <v>15.745637720845901</v>
       </c>
       <c r="F45" s="18">
@@ -4951,14 +4965,14 @@
       <c r="A46" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="39">
+      <c r="B46" s="31">
         <v>234.83314460493301</v>
       </c>
       <c r="C46" s="16">
         <v>234.83314460493301</v>
       </c>
       <c r="D46" s="13"/>
-      <c r="E46" s="42">
+      <c r="E46" s="34">
         <v>15.6555429736622</v>
       </c>
       <c r="F46" s="16">
@@ -5036,14 +5050,14 @@
       <c r="A47" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="41">
+      <c r="B47" s="33">
         <v>170.975653924677</v>
       </c>
       <c r="C47" s="18">
         <v>170.975653924677</v>
       </c>
       <c r="D47" s="19"/>
-      <c r="E47" s="44">
+      <c r="E47" s="36">
         <v>15.5432412658798</v>
       </c>
       <c r="F47" s="18">
@@ -5121,14 +5135,14 @@
       <c r="A48" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="41">
+      <c r="B48" s="33">
         <v>183.78333272544299</v>
       </c>
       <c r="C48" s="18">
         <v>183.78333272544299</v>
       </c>
       <c r="D48" s="19"/>
-      <c r="E48" s="44">
+      <c r="E48" s="36">
         <v>15.315277727120201</v>
       </c>
       <c r="F48" s="18">
@@ -5206,14 +5220,14 @@
       <c r="A49" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="41">
+      <c r="B49" s="33">
         <v>213.98910156718</v>
       </c>
       <c r="C49" s="18">
         <v>213.98910156718</v>
       </c>
       <c r="D49" s="19"/>
-      <c r="E49" s="44">
+      <c r="E49" s="36">
         <v>15.2849358262271</v>
       </c>
       <c r="F49" s="18">
@@ -5291,14 +5305,14 @@
       <c r="A50" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="41">
+      <c r="B50" s="33">
         <v>135.313289613557</v>
       </c>
       <c r="C50" s="18">
         <v>135.313289613557</v>
       </c>
       <c r="D50" s="19"/>
-      <c r="E50" s="44">
+      <c r="E50" s="36">
         <v>15.034809957061899</v>
       </c>
       <c r="F50" s="18">
@@ -5373,31 +5387,31 @@
       <c r="AE50"/>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="41">
+      <c r="B51" s="31">
         <v>222.952658644005</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="16">
         <v>222.952658644005</v>
       </c>
-      <c r="D51" s="19"/>
-      <c r="E51" s="44">
+      <c r="D51" s="13"/>
+      <c r="E51" s="34">
         <v>14.863510576267</v>
       </c>
-      <c r="F51" s="18">
+      <c r="F51" s="16">
         <v>14.863510576267</v>
       </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="21">
+      <c r="G51" s="14"/>
+      <c r="H51" s="15">
         <v>5</v>
       </c>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21">
-        <v>0</v>
-      </c>
-      <c r="K51" s="21">
+      <c r="I51" s="15"/>
+      <c r="J51" s="15">
+        <v>0</v>
+      </c>
+      <c r="K51" s="15">
         <v>0</v>
       </c>
       <c r="L51" s="22">
@@ -5406,13 +5420,13 @@
       <c r="M51" s="22">
         <v>6.3394637003893303E-6</v>
       </c>
-      <c r="N51" s="21">
-        <v>0</v>
-      </c>
-      <c r="O51" s="21">
-        <v>0</v>
-      </c>
-      <c r="P51" s="21">
+      <c r="N51" s="15">
+        <v>0</v>
+      </c>
+      <c r="O51" s="15">
+        <v>0</v>
+      </c>
+      <c r="P51" s="15">
         <v>0</v>
       </c>
       <c r="Q51" s="22">
@@ -5461,14 +5475,14 @@
       <c r="A52" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="41">
+      <c r="B52" s="33">
         <v>177.10454135037901</v>
       </c>
       <c r="C52" s="18">
         <v>177.10454135037901</v>
       </c>
       <c r="D52" s="19"/>
-      <c r="E52" s="44">
+      <c r="E52" s="36">
         <v>14.758711779198201</v>
       </c>
       <c r="F52" s="18">
@@ -5546,14 +5560,14 @@
       <c r="A53" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="41">
+      <c r="B53" s="33">
         <v>189.770698142459</v>
       </c>
       <c r="C53" s="18">
         <v>189.770698142459</v>
       </c>
       <c r="D53" s="19"/>
-      <c r="E53" s="44">
+      <c r="E53" s="36">
         <v>14.5977460109583</v>
       </c>
       <c r="F53" s="18">
@@ -5631,14 +5645,14 @@
       <c r="A54" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="41">
+      <c r="B54" s="33">
         <v>188.58837103182699</v>
       </c>
       <c r="C54" s="18">
         <v>188.58837103182699</v>
       </c>
       <c r="D54" s="19"/>
-      <c r="E54" s="44">
+      <c r="E54" s="36">
         <v>14.506797771679</v>
       </c>
       <c r="F54" s="18">
@@ -5716,14 +5730,14 @@
       <c r="A55" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B55" s="41">
+      <c r="B55" s="33">
         <v>172.79031499130301</v>
       </c>
       <c r="C55" s="18">
         <v>172.79031499130301</v>
       </c>
       <c r="D55" s="19"/>
-      <c r="E55" s="44">
+      <c r="E55" s="36">
         <v>14.399192915941899</v>
       </c>
       <c r="F55" s="18">
@@ -5799,7 +5813,7 @@
     </row>
     <row r="56" spans="1:31" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A57" s="36" t="s">
+      <c r="A57" s="29" t="s">
         <v>77</v>
       </c>
       <c r="B57" s="17"/>
@@ -5829,258 +5843,223 @@
       <c r="Z57" s="17"/>
       <c r="AA57" s="17"/>
       <c r="AB57" s="17"/>
-      <c r="AC57" s="17"/>
+      <c r="AC57" s="30" t="s">
+        <v>76</v>
+      </c>
       <c r="AD57" s="17"/>
-      <c r="AE57" s="37" t="s">
-        <v>76</v>
-      </c>
     </row>
-    <row r="58" spans="1:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="35"/>
-      <c r="M58" s="35"/>
-      <c r="N58" s="35"/>
-      <c r="O58" s="35"/>
-      <c r="P58" s="35"/>
-      <c r="Q58" s="35"/>
-      <c r="R58" s="35"/>
-      <c r="S58" s="35"/>
-      <c r="T58" s="35"/>
-      <c r="U58" s="35"/>
-      <c r="V58" s="35"/>
-      <c r="W58" s="35"/>
-      <c r="X58" s="35"/>
-      <c r="Y58" s="35"/>
-      <c r="Z58" s="35"/>
-      <c r="AA58" s="35"/>
-      <c r="AB58" s="35"/>
-      <c r="AC58" s="35"/>
-      <c r="AD58" s="35"/>
-      <c r="AE58" s="35"/>
+    <row r="58" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="46"/>
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="46"/>
+      <c r="M58" s="46"/>
+      <c r="N58" s="46"/>
+      <c r="O58" s="46"/>
+      <c r="P58" s="46"/>
+      <c r="Q58" s="46"/>
+      <c r="R58" s="46"/>
+      <c r="S58" s="46"/>
+      <c r="T58" s="46"/>
+      <c r="U58" s="46"/>
+      <c r="V58" s="46"/>
+      <c r="W58" s="46"/>
+      <c r="X58" s="46"/>
+      <c r="Y58" s="46"/>
+      <c r="Z58" s="46"/>
+      <c r="AA58" s="46"/>
+      <c r="AB58" s="46"/>
+      <c r="AC58" s="46"/>
+      <c r="AD58" s="46"/>
+      <c r="AE58" s="46"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
+    <row r="59" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="38"/>
-      <c r="I59" s="38"/>
-      <c r="J59" s="38"/>
-      <c r="K59" s="38"/>
-      <c r="L59" s="38"/>
-      <c r="M59" s="38"/>
-      <c r="N59" s="38"/>
-      <c r="O59" s="38"/>
-      <c r="P59" s="38"/>
-      <c r="Q59" s="38"/>
-      <c r="R59" s="38"/>
-      <c r="S59" s="38"/>
-      <c r="T59" s="38"/>
-      <c r="U59" s="38"/>
-      <c r="V59" s="38"/>
-      <c r="W59" s="38"/>
-      <c r="X59" s="38"/>
-      <c r="Y59" s="38"/>
-      <c r="Z59" s="38"/>
-      <c r="AA59" s="38"/>
-      <c r="AB59" s="38"/>
-      <c r="AC59" s="38"/>
-      <c r="AD59" s="38"/>
-      <c r="AE59" s="38"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="46"/>
+      <c r="M59" s="46"/>
+      <c r="N59" s="46"/>
+      <c r="O59" s="46"/>
+      <c r="P59" s="46"/>
+      <c r="Q59" s="46"/>
+      <c r="R59" s="46"/>
+      <c r="S59" s="46"/>
+      <c r="T59" s="46"/>
+      <c r="U59" s="46"/>
+      <c r="V59" s="46"/>
+      <c r="W59" s="46"/>
+      <c r="X59" s="46"/>
+      <c r="Y59" s="46"/>
+      <c r="Z59" s="46"/>
+      <c r="AA59" s="46"/>
+      <c r="AB59" s="46"/>
+      <c r="AC59" s="46"/>
+      <c r="AD59" s="46"/>
+      <c r="AE59" s="46"/>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A60" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" s="38"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="38"/>
-      <c r="I60" s="38"/>
-      <c r="J60" s="38"/>
-      <c r="K60" s="38"/>
-      <c r="L60" s="38"/>
-      <c r="M60" s="38"/>
-      <c r="N60" s="38"/>
-      <c r="O60" s="38"/>
-      <c r="P60" s="38"/>
-      <c r="Q60" s="38"/>
-      <c r="R60" s="38"/>
-      <c r="S60" s="38"/>
-      <c r="T60" s="38"/>
-      <c r="U60" s="38"/>
-      <c r="V60" s="38"/>
-      <c r="W60" s="38"/>
-      <c r="X60" s="38"/>
-      <c r="Y60" s="38"/>
-      <c r="Z60" s="38"/>
-      <c r="AA60" s="38"/>
-      <c r="AB60" s="38"/>
-      <c r="AC60" s="38"/>
-      <c r="AD60" s="38"/>
-      <c r="AE60" s="38"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="39"/>
+      <c r="N60" s="39"/>
+      <c r="O60" s="39"/>
+      <c r="P60" s="39"/>
+      <c r="Q60" s="39"/>
+      <c r="R60" s="39"/>
+      <c r="S60" s="39"/>
+      <c r="T60" s="39"/>
+      <c r="U60" s="39"/>
+      <c r="V60" s="39"/>
+      <c r="W60" s="39"/>
+      <c r="X60" s="39"/>
+      <c r="Y60" s="39"/>
+      <c r="Z60" s="39"/>
+      <c r="AA60" s="39"/>
+      <c r="AB60" s="39"/>
+      <c r="AC60" s="39"/>
+      <c r="AD60" s="39"/>
+      <c r="AE60" s="39"/>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="35"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="35"/>
-      <c r="M61" s="35"/>
-      <c r="N61" s="35"/>
-      <c r="O61" s="35"/>
-      <c r="P61" s="35"/>
-      <c r="Q61" s="35"/>
-      <c r="R61" s="35"/>
-      <c r="S61" s="35"/>
-      <c r="T61" s="35"/>
-      <c r="U61" s="35"/>
-      <c r="V61" s="35"/>
-      <c r="W61" s="35"/>
-      <c r="X61" s="35"/>
-      <c r="Y61" s="35"/>
-      <c r="Z61" s="35"/>
-      <c r="AA61" s="35"/>
-      <c r="AB61" s="35"/>
-      <c r="AC61" s="35"/>
-      <c r="AD61" s="35"/>
-      <c r="AE61" s="35"/>
+      <c r="A61" s="39"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="39"/>
+      <c r="J61" s="39"/>
+      <c r="K61" s="39"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="39"/>
+      <c r="N61" s="39"/>
+      <c r="O61" s="39"/>
+      <c r="P61" s="39"/>
+      <c r="Q61" s="39"/>
+      <c r="R61" s="39"/>
+      <c r="S61" s="39"/>
+      <c r="T61" s="39"/>
+      <c r="U61" s="39"/>
+      <c r="V61" s="39"/>
+      <c r="W61" s="39"/>
+      <c r="X61" s="39"/>
+      <c r="Y61" s="39"/>
+      <c r="Z61" s="39"/>
+      <c r="AA61" s="39"/>
+      <c r="AB61" s="39"/>
+      <c r="AC61" s="39"/>
+      <c r="AD61" s="39"/>
+      <c r="AE61" s="39"/>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="35"/>
-      <c r="K62" s="35"/>
-      <c r="L62" s="35"/>
-      <c r="M62" s="35"/>
-      <c r="N62" s="35"/>
-      <c r="O62" s="35"/>
-      <c r="P62" s="35"/>
-      <c r="Q62" s="35"/>
-      <c r="R62" s="35"/>
-      <c r="S62" s="35"/>
-      <c r="T62" s="35"/>
-      <c r="U62" s="35"/>
-      <c r="V62" s="35"/>
-      <c r="W62" s="35"/>
-      <c r="X62" s="35"/>
-      <c r="Y62" s="35"/>
-      <c r="Z62" s="35"/>
-      <c r="AA62" s="35"/>
-      <c r="AB62" s="35"/>
-      <c r="AC62" s="35"/>
-      <c r="AD62" s="35"/>
-      <c r="AE62" s="35"/>
+      <c r="A62" s="39"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="39"/>
+      <c r="J62" s="39"/>
+      <c r="K62" s="39"/>
+      <c r="L62" s="39"/>
+      <c r="M62" s="39"/>
+      <c r="N62" s="39"/>
+      <c r="O62" s="39"/>
+      <c r="P62" s="39"/>
+      <c r="Q62" s="39"/>
+      <c r="R62" s="39"/>
+      <c r="S62" s="39"/>
+      <c r="T62" s="39"/>
+      <c r="U62" s="39"/>
+      <c r="V62" s="39"/>
+      <c r="W62" s="39"/>
+      <c r="X62" s="39"/>
+      <c r="Y62" s="39"/>
+      <c r="Z62" s="39"/>
+      <c r="AA62" s="39"/>
+      <c r="AB62" s="39"/>
+      <c r="AC62" s="39"/>
+      <c r="AD62" s="39"/>
+      <c r="AE62" s="39"/>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="35"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="35"/>
-      <c r="O63" s="35"/>
-      <c r="P63" s="35"/>
-      <c r="Q63" s="35"/>
-      <c r="R63" s="35"/>
-      <c r="S63" s="35"/>
-      <c r="T63" s="35"/>
-      <c r="U63" s="35"/>
-      <c r="V63" s="35"/>
-      <c r="W63" s="35"/>
-      <c r="X63" s="35"/>
-      <c r="Y63" s="35"/>
-      <c r="Z63" s="35"/>
-      <c r="AA63" s="35"/>
-      <c r="AB63" s="35"/>
-      <c r="AC63" s="35"/>
-      <c r="AD63" s="35"/>
-      <c r="AE63" s="35"/>
-    </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A64" s="35"/>
-      <c r="B64" s="35"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="35"/>
-      <c r="I64" s="35"/>
-      <c r="J64" s="35"/>
-      <c r="K64" s="35"/>
-      <c r="L64" s="35"/>
-      <c r="M64" s="35"/>
-      <c r="N64" s="35"/>
-      <c r="O64" s="35"/>
-      <c r="P64" s="35"/>
-      <c r="Q64" s="35"/>
-      <c r="R64" s="35"/>
-      <c r="S64" s="35"/>
-      <c r="T64" s="35"/>
-      <c r="U64" s="35"/>
-      <c r="V64" s="35"/>
-      <c r="W64" s="35"/>
-      <c r="X64" s="35"/>
-      <c r="Y64" s="35"/>
-      <c r="Z64" s="35"/>
-      <c r="AA64" s="35"/>
-      <c r="AB64" s="35"/>
-      <c r="AC64" s="35"/>
-      <c r="AD64" s="35"/>
-      <c r="AE64" s="35"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="39"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="39"/>
+      <c r="L63" s="39"/>
+      <c r="M63" s="39"/>
+      <c r="N63" s="39"/>
+      <c r="O63" s="39"/>
+      <c r="P63" s="39"/>
+      <c r="Q63" s="39"/>
+      <c r="R63" s="39"/>
+      <c r="S63" s="39"/>
+      <c r="T63" s="39"/>
+      <c r="U63" s="39"/>
+      <c r="V63" s="39"/>
+      <c r="W63" s="39"/>
+      <c r="X63" s="39"/>
+      <c r="Y63" s="39"/>
+      <c r="Z63" s="39"/>
+      <c r="AA63" s="39"/>
+      <c r="AB63" s="39"/>
+      <c r="AC63" s="39"/>
+      <c r="AD63" s="39"/>
+      <c r="AE63" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
+    <mergeCell ref="A60:AE60"/>
     <mergeCell ref="A61:AE61"/>
     <mergeCell ref="A62:AE62"/>
     <mergeCell ref="A63:AE63"/>
-    <mergeCell ref="A64:AE64"/>
     <mergeCell ref="A1:AE1"/>
     <mergeCell ref="A2:AE2"/>
     <mergeCell ref="A58:AE58"/>
     <mergeCell ref="A59:AE59"/>
-    <mergeCell ref="A60:AE60"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="H4:H5"/>
@@ -6133,6 +6112,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="3" scale="73" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>